<commit_message>
Change RHFF to switch to electricity instead of hydrogen
</commit_message>
<xml_diff>
--- a/InputData/dist-heat/RHFF/Recipient Heat Fuel Fractions.xlsx
+++ b/InputData/dist-heat/RHFF/Recipient Heat Fuel Fractions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipM\InputData\dist-heat\RHFFfC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\dist-heat\RHFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4A5C5A-F1DD-4AB6-ABF0-1E0279B2EC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="11055"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Source:</t>
   </si>
@@ -49,9 +50,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>electricity would be inefficient, relative to the end users using electricity for heat directly).</t>
-  </si>
-  <si>
     <t>crude oil</t>
   </si>
   <si>
@@ -64,9 +62,6 @@
     <t>hydrogen</t>
   </si>
   <si>
-    <t>District heat facilities most likely need to burn thermal fuels to generate heat (as using</t>
-  </si>
-  <si>
     <t>to Other Fuels policy.</t>
   </si>
   <si>
@@ -79,19 +74,13 @@
     <t>To type (below)  / From type (right)</t>
   </si>
   <si>
-    <t>For the United States, where most district heat facilities currently burn natural gas, we</t>
-  </si>
-  <si>
-    <t>specify this policy lever as a shift to hydrogen, as one of the only thermal fuel options</t>
-  </si>
-  <si>
-    <t>to further reduce GHG emissions.</t>
+    <t>We assume shifting to electricity via large scale electric heat pumps.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,10 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -140,9 +128,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -163,9 +148,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,9 +188,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -448,10 +433,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -460,7 +447,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,13 +464,13 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
+      <c r="A6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
+      <c r="A7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -491,30 +478,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -524,122 +488,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="11" width="15" style="5" customWidth="1"/>
+    <col min="2" max="11" width="15" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0</v>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -647,34 +613,34 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
         <v>0</v>
       </c>
     </row>
@@ -682,34 +648,34 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -717,34 +683,34 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
         <v>0</v>
       </c>
     </row>
@@ -752,175 +718,175 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>